<commit_message>
Update on Base page
</commit_message>
<xml_diff>
--- a/ESF/Resources/TestData/Testdata1.xlsx
+++ b/ESF/Resources/TestData/Testdata1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>Email</t>
   </si>
@@ -146,6 +146,30 @@
   </si>
   <si>
     <t>Atanu_Step_670</t>
+  </si>
+  <si>
+    <t>Atanu_Step_684</t>
+  </si>
+  <si>
+    <t>Atanu_Step_136</t>
+  </si>
+  <si>
+    <t>Atanu_Step_935</t>
+  </si>
+  <si>
+    <t>Atanu_Step_816</t>
+  </si>
+  <si>
+    <t>Atanu_Step_49</t>
+  </si>
+  <si>
+    <t>Atanu_Test_152</t>
+  </si>
+  <si>
+    <t>Atanu_Test_940</t>
+  </si>
+  <si>
+    <t>Atanu_Step_245</t>
   </si>
 </sst>
 </file>
@@ -1195,7 +1219,7 @@
         <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1281,7 +1305,7 @@
         <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modify code in every pages
</commit_message>
<xml_diff>
--- a/ESF/Resources/TestData/Testdata1.xlsx
+++ b/ESF/Resources/TestData/Testdata1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="92">
   <si>
     <t>Email</t>
   </si>
@@ -223,6 +223,78 @@
   </si>
   <si>
     <t>test_field122</t>
+  </si>
+  <si>
+    <t>Atanu_Test_134</t>
+  </si>
+  <si>
+    <t>Atanu_Test_73</t>
+  </si>
+  <si>
+    <t>Atanu_Test_312</t>
+  </si>
+  <si>
+    <t>Atanu_Step_813</t>
+  </si>
+  <si>
+    <t>Atanu_Step_39</t>
+  </si>
+  <si>
+    <t>Atanu_Step_143</t>
+  </si>
+  <si>
+    <t>Atanu_Step_482</t>
+  </si>
+  <si>
+    <t>Test_Section_327</t>
+  </si>
+  <si>
+    <t>Atanu_Test_657</t>
+  </si>
+  <si>
+    <t>Atanu_Test_536</t>
+  </si>
+  <si>
+    <t>Atanu_Test_802</t>
+  </si>
+  <si>
+    <t>Atanu_Step_322</t>
+  </si>
+  <si>
+    <t>Atanu_Test_166</t>
+  </si>
+  <si>
+    <t>Atanu_Test_835</t>
+  </si>
+  <si>
+    <t>Atanu_Test_338</t>
+  </si>
+  <si>
+    <t>Atanu_Test_544</t>
+  </si>
+  <si>
+    <t>Atanu_Step_978</t>
+  </si>
+  <si>
+    <t>Test_Section_421</t>
+  </si>
+  <si>
+    <t>Test_Section_787</t>
+  </si>
+  <si>
+    <t>Test_Section_304</t>
+  </si>
+  <si>
+    <t>Test_Section_456</t>
+  </si>
+  <si>
+    <t>Test_Section_384</t>
+  </si>
+  <si>
+    <t>Test_Section_138</t>
+  </si>
+  <si>
+    <t>user_name_771</t>
   </si>
 </sst>
 </file>
@@ -1199,8 +1271,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="27.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="19.5714285714286" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="27.7142857142857" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.5714285714286" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1236,12 +1308,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="22.7142857142857" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.5714285714286" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.1428571428571" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.2857142857143" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.4285714285714" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="22.7142857142857" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.5714285714286" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.1428571428571" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.2857142857143" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.4285714285714" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="1" spans="1:6">
@@ -1281,7 +1353,7 @@
         <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1301,15 +1373,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="21.2857142857143" customWidth="1"/>
-    <col min="3" max="3" width="27.4285714285714" customWidth="1"/>
-    <col min="4" max="4" width="21.4285714285714" customWidth="1"/>
-    <col min="5" max="5" width="19.8571428571429" customWidth="1"/>
-    <col min="6" max="6" width="25.2857142857143" customWidth="1"/>
-    <col min="7" max="7" width="18.8571428571429" customWidth="1"/>
-    <col min="8" max="8" width="19.8571428571429" customWidth="1"/>
-    <col min="9" max="9" width="27.4285714285714" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.2857142857143" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.4285714285714" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.4285714285714" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.8571428571429" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="25.2857142857143" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="18.8571428571429" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="19.8571428571429" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="27.4285714285714" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="1" ht="17.25" spans="1:9">
@@ -1367,7 +1439,7 @@
         <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>30</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1390,7 +1462,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.7142857142857" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.7142857142857" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1466,15 +1538,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="22.2857142857143" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="24.2857142857143" customWidth="1"/>
-    <col min="5" max="5" width="27.5714285714286" customWidth="1"/>
-    <col min="6" max="6" width="27.1428571428571" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="18.5714285714286" customWidth="1"/>
-    <col min="9" max="9" width="27.2857142857143" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.2857142857143" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="24.2857142857143" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="27.5714285714286" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.1428571428571" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="18.5714285714286" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="27.2857142857143" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" spans="1:9">
@@ -1532,7 +1604,7 @@
         <v>40</v>
       </c>
       <c r="I2" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1546,30 +1618,30 @@
   <sheetPr/>
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="17.1428571428571" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.2857142857143" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="25.8571428571429" customWidth="1"/>
-    <col min="6" max="6" width="17.5714285714286" customWidth="1"/>
-    <col min="7" max="7" width="19.1428571428571" customWidth="1"/>
-    <col min="8" max="8" width="26.5714285714286" customWidth="1"/>
-    <col min="9" max="9" width="24.2857142857143" customWidth="1"/>
-    <col min="10" max="10" width="27.7142857142857" customWidth="1"/>
-    <col min="11" max="11" width="23.4285714285714" customWidth="1"/>
-    <col min="12" max="12" width="19" customWidth="1"/>
-    <col min="13" max="13" width="19.8571428571429" customWidth="1"/>
-    <col min="14" max="14" width="20" customWidth="1"/>
-    <col min="15" max="15" width="24.1428571428571" customWidth="1"/>
-    <col min="16" max="16" width="18.4285714285714" customWidth="1"/>
-    <col min="17" max="17" width="19.8571428571429" customWidth="1"/>
-    <col min="18" max="18" width="27.7142857142857" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.1428571428571" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.2857142857143" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="25.8571428571429" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.5714285714286" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="19.1428571428571" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="26.5714285714286" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="24.2857142857143" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="27.7142857142857" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.4285714285714" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="19.8571428571429" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="24.1428571428571" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="18.4285714285714" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="19.8571428571429" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="27.7142857142857" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">

</xml_diff>

<commit_message>
Optimize code in every page
</commit_message>
<xml_diff>
--- a/ESF/Resources/TestData/Testdata1.xlsx
+++ b/ESF/Resources/TestData/Testdata1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20370" windowHeight="7665" firstSheet="1" activeTab="5"/>
+    <workbookView windowWidth="20370" windowHeight="7665" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="71">
   <si>
     <t>Email</t>
   </si>
@@ -63,7 +63,7 @@
     <t>atanu</t>
   </si>
   <si>
-    <t>Atanu_Test_940</t>
+    <t>Atanu_Test_544</t>
   </si>
   <si>
     <t>Application Step Name</t>
@@ -111,7 +111,7 @@
     <t>single_column</t>
   </si>
   <si>
-    <t>Atanu_Step_245</t>
+    <t>Atanu_Step_766</t>
   </si>
   <si>
     <t>Section Number</t>
@@ -144,7 +144,7 @@
     <t>test</t>
   </si>
   <si>
-    <t>Test_Section_609</t>
+    <t>Test_Section_647</t>
   </si>
   <si>
     <t>Unique Id</t>
@@ -225,76 +225,13 @@
     <t>test_field122</t>
   </si>
   <si>
-    <t>Atanu_Test_134</t>
-  </si>
-  <si>
-    <t>Atanu_Test_73</t>
-  </si>
-  <si>
-    <t>Atanu_Test_312</t>
-  </si>
-  <si>
-    <t>Atanu_Step_813</t>
-  </si>
-  <si>
-    <t>Atanu_Step_39</t>
-  </si>
-  <si>
-    <t>Atanu_Step_143</t>
-  </si>
-  <si>
-    <t>Atanu_Step_482</t>
-  </si>
-  <si>
-    <t>Test_Section_327</t>
-  </si>
-  <si>
-    <t>Atanu_Test_657</t>
-  </si>
-  <si>
-    <t>Atanu_Test_536</t>
-  </si>
-  <si>
-    <t>Atanu_Test_802</t>
-  </si>
-  <si>
-    <t>Atanu_Step_322</t>
-  </si>
-  <si>
-    <t>Atanu_Test_166</t>
-  </si>
-  <si>
-    <t>Atanu_Test_835</t>
-  </si>
-  <si>
-    <t>Atanu_Test_338</t>
-  </si>
-  <si>
-    <t>Atanu_Test_544</t>
-  </si>
-  <si>
-    <t>Atanu_Step_978</t>
-  </si>
-  <si>
-    <t>Test_Section_421</t>
-  </si>
-  <si>
-    <t>Test_Section_787</t>
-  </si>
-  <si>
-    <t>Test_Section_304</t>
-  </si>
-  <si>
-    <t>Test_Section_456</t>
-  </si>
-  <si>
-    <t>Test_Section_384</t>
-  </si>
-  <si>
-    <t>Test_Section_138</t>
-  </si>
-  <si>
-    <t>user_name_771</t>
+    <t>user_name_275</t>
+  </si>
+  <si>
+    <t>Test_Section_675</t>
+  </si>
+  <si>
+    <t>Test_Section_375</t>
   </si>
 </sst>
 </file>
@@ -302,10 +239,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -338,6 +275,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -345,15 +304,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -367,25 +335,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -397,42 +359,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -445,22 +397,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -475,91 +412,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -577,85 +592,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -672,8 +609,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -689,17 +641,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -730,24 +671,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -766,157 +694,166 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -924,9 +861,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -1276,18 +1210,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="7">
         <v>123456</v>
       </c>
     </row>
@@ -1316,20 +1250,20 @@
     <col min="6" max="6" customWidth="true" width="34.4285714285714" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="1" spans="1:6">
-      <c r="A1" s="5" t="s">
+    <row r="1" s="4" customFormat="1" spans="1:6">
+      <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F1" t="s">
@@ -1337,23 +1271,23 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1367,8 +1301,8 @@
   <sheetPr/>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1384,62 +1318,62 @@
     <col min="9" max="9" customWidth="true" width="27.4285714285714" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="1" ht="17.25" spans="1:9">
-      <c r="A1" s="6" t="s">
+    <row r="1" s="4" customFormat="1" ht="17.25" spans="1:9">
+      <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" s="5" customFormat="1" spans="1:9">
+    <row r="2" s="4" customFormat="1" spans="1:9">
       <c r="A2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>91</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1471,55 +1405,55 @@
       </c>
     </row>
     <row r="2" ht="17.25" spans="1:1">
-      <c r="A2" s="4"/>
+      <c r="A2" s="3"/>
     </row>
     <row r="3" ht="17.25" spans="1:1">
-      <c r="A3" s="4"/>
+      <c r="A3" s="3"/>
     </row>
     <row r="4" ht="17.25" spans="1:1">
-      <c r="A4" s="4"/>
+      <c r="A4" s="3"/>
     </row>
     <row r="5" ht="17.25" spans="1:1">
-      <c r="A5" s="4"/>
+      <c r="A5" s="3"/>
     </row>
     <row r="6" ht="17.25" spans="1:1">
-      <c r="A6" s="4"/>
+      <c r="A6" s="3"/>
     </row>
     <row r="7" ht="17.25" spans="1:1">
-      <c r="A7" s="4"/>
+      <c r="A7" s="3"/>
     </row>
     <row r="8" ht="17.25" spans="1:1">
-      <c r="A8" s="4"/>
+      <c r="A8" s="3"/>
     </row>
     <row r="9" ht="17.25" spans="1:1">
-      <c r="A9" s="4"/>
+      <c r="A9" s="3"/>
     </row>
     <row r="10" ht="17.25" spans="1:1">
-      <c r="A10" s="4"/>
+      <c r="A10" s="3"/>
     </row>
     <row r="11" ht="17.25" spans="1:1">
-      <c r="A11" s="4"/>
+      <c r="A11" s="3"/>
     </row>
     <row r="12" ht="17.25" spans="1:1">
-      <c r="A12" s="4"/>
+      <c r="A12" s="3"/>
     </row>
     <row r="13" ht="17.25" spans="1:1">
-      <c r="A13" s="4"/>
+      <c r="A13" s="3"/>
     </row>
     <row r="14" ht="17.25" spans="1:1">
-      <c r="A14" s="4"/>
+      <c r="A14" s="3"/>
     </row>
     <row r="15" ht="17.25" spans="1:1">
-      <c r="A15" s="4"/>
+      <c r="A15" s="3"/>
     </row>
     <row r="16" ht="17.25" spans="1:1">
-      <c r="A16" s="4"/>
+      <c r="A16" s="3"/>
     </row>
     <row r="17" ht="17.25" spans="1:1">
-      <c r="A17" s="4"/>
+      <c r="A17" s="3"/>
     </row>
     <row r="18" ht="17.25" spans="1:1">
-      <c r="A18" s="4"/>
+      <c r="A18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1556,7 +1490,7 @@
       <c r="B1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D1" t="s">
@@ -1578,33 +1512,33 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" s="3" customFormat="1" spans="1:9">
-      <c r="A2" s="3">
+    <row r="2" s="1" customFormat="1" spans="1:9">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>40</v>
       </c>
       <c r="I2" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1618,8 +1552,8 @@
   <sheetPr/>
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1700,7 +1634,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:17">
+    <row r="2" s="1" customFormat="1" spans="1:18">
       <c r="A2" s="1" t="s">
         <v>56</v>
       </c>
@@ -1751,6 +1685,9 @@
       </c>
       <c r="Q2" s="1" t="s">
         <v>67</v>
+      </c>
+      <c r="R2" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Block and Block Field
</commit_message>
<xml_diff>
--- a/ESF/Resources/TestData/Testdata1.xlsx
+++ b/ESF/Resources/TestData/Testdata1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="1" activeTab="6"/>
+    <workbookView windowWidth="28800" windowHeight="12495" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="Section_Details" sheetId="5" r:id="rId5"/>
     <sheet name="Field_Details" sheetId="6" r:id="rId6"/>
     <sheet name="Condition_Details" sheetId="7" r:id="rId7"/>
+    <sheet name="Block_Details" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="121">
   <si>
     <t>Email</t>
   </si>
@@ -278,6 +279,111 @@
   </si>
   <si>
     <t>( Condition2 )</t>
+  </si>
+  <si>
+    <t>Application Block Name</t>
+  </si>
+  <si>
+    <t>Block Type</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Modified Block Name</t>
+  </si>
+  <si>
+    <t>genericBlock</t>
+  </si>
+  <si>
+    <t>This is generic block type desc</t>
+  </si>
+  <si>
+    <t>col-mo-10</t>
+  </si>
+  <si>
+    <t>cutom-10-name</t>
+  </si>
+  <si>
+    <t>test_field</t>
+  </si>
+  <si>
+    <t>Atanu_Test_973</t>
+  </si>
+  <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t>This is menu block type desc</t>
+  </si>
+  <si>
+    <t>cutom-10</t>
+  </si>
+  <si>
+    <t>Atanu_Test_225</t>
+  </si>
+  <si>
+    <t>Atanu_Step_541</t>
+  </si>
+  <si>
+    <t>Test_Section_101</t>
+  </si>
+  <si>
+    <t>user_name_373</t>
+  </si>
+  <si>
+    <t>user_name_188</t>
+  </si>
+  <si>
+    <t>user_name_596</t>
+  </si>
+  <si>
+    <t>user_name_708</t>
+  </si>
+  <si>
+    <t>user_name_308</t>
+  </si>
+  <si>
+    <t>user_name_180</t>
+  </si>
+  <si>
+    <t>user_name_727</t>
+  </si>
+  <si>
+    <t>user_name_706</t>
+  </si>
+  <si>
+    <t>user_name_186</t>
+  </si>
+  <si>
+    <t>user_name_802</t>
+  </si>
+  <si>
+    <t>user_name_463</t>
+  </si>
+  <si>
+    <t>user_name_668</t>
+  </si>
+  <si>
+    <t>user_name_664</t>
+  </si>
+  <si>
+    <t>user_name_283</t>
+  </si>
+  <si>
+    <t>Atanu_Step_740</t>
+  </si>
+  <si>
+    <t>Test_Section_563</t>
+  </si>
+  <si>
+    <t>user_name_692</t>
+  </si>
+  <si>
+    <t>Atanu_Test_629</t>
+  </si>
+  <si>
+    <t>user_name_20</t>
   </si>
 </sst>
 </file>
@@ -285,10 +391,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -321,13 +427,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -340,6 +440,29 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -358,14 +481,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -381,14 +496,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -399,6 +506,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -421,22 +542,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -458,37 +564,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -500,66 +726,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -572,73 +738,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -654,9 +760,20 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -676,15 +793,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -696,6 +804,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -738,164 +855,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1251,8 +1357,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="27.7142857142857" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.5714285714286" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="27.7142857142857" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.5714285714286" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1280,20 +1386,20 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="22.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="18.5714285714286" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="21.1428571428571" customWidth="1"/>
-    <col min="5" max="5" width="19.2857142857143" customWidth="1"/>
-    <col min="6" max="6" width="34.4285714285714" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="22.7142857142857" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.5714285714286" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.1428571428571" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.2857142857143" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.4285714285714" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="1" spans="1:6">
@@ -1333,6 +1439,26 @@
         <v>13</v>
       </c>
       <c r="F2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1347,21 +1473,21 @@
   <sheetPr/>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="21.2857142857143" customWidth="1"/>
-    <col min="3" max="3" width="27.4285714285714" customWidth="1"/>
-    <col min="4" max="4" width="21.4285714285714" customWidth="1"/>
-    <col min="5" max="5" width="19.8571428571429" customWidth="1"/>
-    <col min="6" max="6" width="25.2857142857143" customWidth="1"/>
-    <col min="7" max="7" width="18.8571428571429" customWidth="1"/>
-    <col min="8" max="8" width="19.8571428571429" customWidth="1"/>
-    <col min="9" max="9" width="27.4285714285714" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.2857142857143" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.4285714285714" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.4285714285714" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.8571428571429" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="25.2857142857143" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="18.8571428571429" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="19.8571428571429" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="27.4285714285714" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="1" ht="17.25" spans="1:9">
@@ -1419,7 +1545,7 @@
         <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>30</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1442,7 +1568,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.7142857142857" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.7142857142857" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1518,15 +1644,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.2857142857143" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.2857142857143" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="27.5714285714286" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.1428571428571" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.5714285714286" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="27.2857142857143" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.2857142857143" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="24.2857142857143" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="27.5714285714286" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.1428571428571" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="18.5714285714286" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="27.2857142857143" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" spans="1:9">
@@ -1584,7 +1710,7 @@
         <v>40</v>
       </c>
       <c r="I2" t="s">
-        <v>41</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1604,24 +1730,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="17.1428571428571" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.2857142857143" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="25.8571428571429" customWidth="1"/>
-    <col min="6" max="6" width="17.5714285714286" customWidth="1"/>
-    <col min="7" max="7" width="19.1428571428571" customWidth="1"/>
-    <col min="8" max="8" width="26.5714285714286" customWidth="1"/>
-    <col min="9" max="9" width="24.2857142857143" customWidth="1"/>
-    <col min="10" max="10" width="27.7142857142857" customWidth="1"/>
-    <col min="11" max="11" width="23.4285714285714" customWidth="1"/>
-    <col min="12" max="12" width="19" customWidth="1"/>
-    <col min="13" max="13" width="19.8571428571429" customWidth="1"/>
-    <col min="14" max="14" width="20" customWidth="1"/>
-    <col min="15" max="15" width="24.1428571428571" customWidth="1"/>
-    <col min="16" max="16" width="18.4285714285714" customWidth="1"/>
-    <col min="17" max="17" width="19.8571428571429" customWidth="1"/>
-    <col min="18" max="18" width="27.7142857142857" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.1428571428571" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.2857142857143" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="25.8571428571429" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.5714285714286" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="19.1428571428571" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="26.5714285714286" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="24.2857142857143" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="27.7142857142857" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.4285714285714" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="19.8571428571429" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="24.1428571428571" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="18.4285714285714" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="19.8571428571429" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="27.7142857142857" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -1733,7 +1859,7 @@
         <v>67</v>
       </c>
       <c r="R2" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1750,22 +1876,22 @@
   <sheetPr/>
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="20.4285714285714" customWidth="1"/>
-    <col min="2" max="2" width="20.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="21.5714285714286" customWidth="1"/>
-    <col min="5" max="5" width="20.8571428571429" customWidth="1"/>
-    <col min="6" max="6" width="27.2857142857143" customWidth="1"/>
-    <col min="7" max="7" width="24.2857142857143" customWidth="1"/>
-    <col min="8" max="8" width="18.7142857142857" customWidth="1"/>
-    <col min="9" max="9" width="22.7142857142857" customWidth="1"/>
-    <col min="10" max="10" width="31.4285714285714" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="20.4285714285714" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.1428571428571" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.5714285714286" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="20.8571428571429" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.2857142857143" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="24.2857142857143" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="18.7142857142857" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="22.7142857142857" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="31.4285714285714" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1836,7 +1962,6 @@
       <c r="C3" t="s">
         <v>30</v>
       </c>
-      <c r="D3"/>
       <c r="E3" t="s">
         <v>68</v>
       </c>
@@ -1851,6 +1976,109 @@
       </c>
       <c r="I3" t="s">
         <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="22.7142857142857" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.1428571428571" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="36.4285714285714" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="33.8571428571429" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Message and Workflow
</commit_message>
<xml_diff>
--- a/ESF/Resources/TestData/Testdata1.xlsx
+++ b/ESF/Resources/TestData/Testdata1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12495" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="19890" windowHeight="7665" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,15 @@
     <sheet name="Field_Details" sheetId="6" r:id="rId6"/>
     <sheet name="Condition_Details" sheetId="7" r:id="rId7"/>
     <sheet name="Block_Details" sheetId="8" r:id="rId8"/>
+    <sheet name="Message_Details" sheetId="9" r:id="rId9"/>
+    <sheet name="Workflow_Details" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="128">
   <si>
     <t>Email</t>
   </si>
@@ -113,159 +115,165 @@
     <t>single_column</t>
   </si>
   <si>
+    <t>Atanu_Step_751</t>
+  </si>
+  <si>
+    <t>Section Number</t>
+  </si>
+  <si>
+    <t>Section Name</t>
+  </si>
+  <si>
+    <t>Sequence Number</t>
+  </si>
+  <si>
+    <t>Section Class Name</t>
+  </si>
+  <si>
+    <t>Modified Section Name</t>
+  </si>
+  <si>
+    <t>Test_Section</t>
+  </si>
+  <si>
+    <t>col-mo-12</t>
+  </si>
+  <si>
+    <t>col-mo-6</t>
+  </si>
+  <si>
+    <t>custom-class</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Test_Section_563</t>
+  </si>
+  <si>
+    <t>Unique Id</t>
+  </si>
+  <si>
+    <t>Field Label</t>
+  </si>
+  <si>
+    <t>Field Type</t>
+  </si>
+  <si>
+    <t>Field Sequence</t>
+  </si>
+  <si>
+    <t>Placeholder Text</t>
+  </si>
+  <si>
+    <t>Tooltip</t>
+  </si>
+  <si>
+    <t>Field Character Limit</t>
+  </si>
+  <si>
+    <t>API Key</t>
+  </si>
+  <si>
+    <t>Request API Key</t>
+  </si>
+  <si>
+    <t>Response API Key</t>
+  </si>
+  <si>
+    <t>CSS Class Name</t>
+  </si>
+  <si>
+    <t>Default Value</t>
+  </si>
+  <si>
+    <t>Possible Values</t>
+  </si>
+  <si>
+    <t>Modified Uniq Id</t>
+  </si>
+  <si>
+    <t>user_name</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Textfield</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter Your Username </t>
+  </si>
+  <si>
+    <t>Username needed</t>
+  </si>
+  <si>
+    <t>http#:/#api-key</t>
+  </si>
+  <si>
+    <t>http#:/#Requestapi-key</t>
+  </si>
+  <si>
+    <t>Responseapi-key</t>
+  </si>
+  <si>
+    <t>Bootstrap</t>
+  </si>
+  <si>
+    <t>col-6</t>
+  </si>
+  <si>
+    <t>Comparison Field</t>
+  </si>
+  <si>
+    <t>test_field122</t>
+  </si>
+  <si>
+    <t>user_name_20</t>
+  </si>
+  <si>
+    <t>Condition Name</t>
+  </si>
+  <si>
+    <t>Condition ID</t>
+  </si>
+  <si>
+    <t>Step Name</t>
+  </si>
+  <si>
+    <t>Block Name</t>
+  </si>
+  <si>
+    <t>Field Unique Id</t>
+  </si>
+  <si>
+    <t>Comparison Operator</t>
+  </si>
+  <si>
+    <t>Field Values</t>
+  </si>
+  <si>
+    <t>Api Key</t>
+  </si>
+  <si>
+    <t>Query</t>
+  </si>
+  <si>
+    <t>Modified Condition Id</t>
+  </si>
+  <si>
+    <t>Test_Condition</t>
+  </si>
+  <si>
+    <t>Condition1</t>
+  </si>
+  <si>
     <t>Atanu_Step_684</t>
   </si>
   <si>
-    <t>Section Number</t>
-  </si>
-  <si>
-    <t>Section Name</t>
-  </si>
-  <si>
-    <t>Sequence Number</t>
-  </si>
-  <si>
-    <t>Section Class Name</t>
-  </si>
-  <si>
-    <t>Modified Section Name</t>
-  </si>
-  <si>
-    <t>Test_Section</t>
-  </si>
-  <si>
-    <t>col-mo-12</t>
-  </si>
-  <si>
-    <t>col-mo-6</t>
-  </si>
-  <si>
-    <t>custom-class</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>Test_Section_375</t>
-  </si>
-  <si>
-    <t>Unique Id</t>
-  </si>
-  <si>
-    <t>Field Label</t>
-  </si>
-  <si>
-    <t>Field Type</t>
-  </si>
-  <si>
-    <t>Field Sequence</t>
-  </si>
-  <si>
-    <t>Placeholder Text</t>
-  </si>
-  <si>
-    <t>Tooltip</t>
-  </si>
-  <si>
-    <t>Field Character Limit</t>
-  </si>
-  <si>
-    <t>API Key</t>
-  </si>
-  <si>
-    <t>Request API Key</t>
-  </si>
-  <si>
-    <t>Response API Key</t>
-  </si>
-  <si>
-    <t>CSS Class Name</t>
-  </si>
-  <si>
-    <t>Default Value</t>
-  </si>
-  <si>
-    <t>Possible Values</t>
-  </si>
-  <si>
-    <t>Modified Uniq Id</t>
-  </si>
-  <si>
-    <t>user_name</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Textfield</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enter Your Username </t>
-  </si>
-  <si>
-    <t>Username needed</t>
-  </si>
-  <si>
-    <t>http#:/#api-key</t>
-  </si>
-  <si>
-    <t>http#:/#Requestapi-key</t>
-  </si>
-  <si>
-    <t>Responseapi-key</t>
-  </si>
-  <si>
-    <t>Bootstrap</t>
-  </si>
-  <si>
-    <t>col-6</t>
-  </si>
-  <si>
-    <t>Comparison Field</t>
-  </si>
-  <si>
-    <t>test_field122</t>
-  </si>
-  <si>
     <t>user_name_275</t>
   </si>
   <si>
-    <t>Condition Name</t>
-  </si>
-  <si>
-    <t>Condition ID</t>
-  </si>
-  <si>
-    <t>Step Name</t>
-  </si>
-  <si>
-    <t>Block Name</t>
-  </si>
-  <si>
-    <t>Field Unique Id</t>
-  </si>
-  <si>
-    <t>Comparison Operator</t>
-  </si>
-  <si>
-    <t>Field Values</t>
-  </si>
-  <si>
-    <t>Api Key</t>
-  </si>
-  <si>
-    <t>Query</t>
-  </si>
-  <si>
-    <t>Modified Condition Id</t>
-  </si>
-  <si>
-    <t>Test_Condition</t>
-  </si>
-  <si>
-    <t>Condition1</t>
-  </si>
-  <si>
     <t>NE</t>
   </si>
   <si>
@@ -320,73 +328,85 @@
     <t>cutom-10</t>
   </si>
   <si>
-    <t>Atanu_Test_225</t>
-  </si>
-  <si>
-    <t>Atanu_Step_541</t>
-  </si>
-  <si>
-    <t>Test_Section_101</t>
-  </si>
-  <si>
-    <t>user_name_373</t>
-  </si>
-  <si>
-    <t>user_name_188</t>
-  </si>
-  <si>
-    <t>user_name_596</t>
-  </si>
-  <si>
-    <t>user_name_708</t>
-  </si>
-  <si>
-    <t>user_name_308</t>
-  </si>
-  <si>
-    <t>user_name_180</t>
-  </si>
-  <si>
-    <t>user_name_727</t>
-  </si>
-  <si>
-    <t>user_name_706</t>
-  </si>
-  <si>
-    <t>user_name_186</t>
-  </si>
-  <si>
-    <t>user_name_802</t>
-  </si>
-  <si>
-    <t>user_name_463</t>
-  </si>
-  <si>
-    <t>user_name_668</t>
-  </si>
-  <si>
-    <t>user_name_664</t>
-  </si>
-  <si>
-    <t>user_name_283</t>
-  </si>
-  <si>
-    <t>Atanu_Step_740</t>
-  </si>
-  <si>
-    <t>Test_Section_563</t>
-  </si>
-  <si>
-    <t>user_name_692</t>
-  </si>
-  <si>
     <t>Atanu_Test_629</t>
   </si>
   <si>
-    <t>user_name_20</t>
-  </si>
-  <si>
-    <t>Atanu_Step_602</t>
+    <t>Enter a message code</t>
+  </si>
+  <si>
+    <t>Select a message type</t>
+  </si>
+  <si>
+    <t>Enter the message to be displayed</t>
+  </si>
+  <si>
+    <t>Modified Message Code</t>
+  </si>
+  <si>
+    <t>atanu_test_message</t>
+  </si>
+  <si>
+    <t>Static Message Text</t>
+  </si>
+  <si>
+    <t>This message is for testing perpose</t>
+  </si>
+  <si>
+    <t>atanu_test_message_631</t>
+  </si>
+  <si>
+    <t>Name of the workflow</t>
+  </si>
+  <si>
+    <t>Associate Progress Bar</t>
+  </si>
+  <si>
+    <t>Step Count Color</t>
+  </si>
+  <si>
+    <t>Percentage Text Color</t>
+  </si>
+  <si>
+    <t>Progress Bar Color</t>
+  </si>
+  <si>
+    <t>Modified Workflow Name</t>
+  </si>
+  <si>
+    <t>Test_Workflow</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Atanu_Step_393</t>
+  </si>
+  <si>
+    <t>Test_Workflow_319</t>
+  </si>
+  <si>
+    <t>Test_Workflow_610</t>
+  </si>
+  <si>
+    <t>Test_Workflow_315</t>
+  </si>
+  <si>
+    <t>Test_Workflow_491</t>
+  </si>
+  <si>
+    <t>Test_Workflow_196</t>
+  </si>
+  <si>
+    <t>Test_Workflow_347</t>
+  </si>
+  <si>
+    <t>Test_Workflow_515</t>
   </si>
 </sst>
 </file>
@@ -395,9 +415,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -430,7 +450,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -440,24 +459,24 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -470,17 +489,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -507,6 +526,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -515,22 +550,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -545,14 +572,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -567,187 +587,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -761,22 +781,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -792,6 +807,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -820,6 +844,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -835,21 +870,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -863,18 +883,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -884,28 +904,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -914,97 +934,97 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1386,12 +1406,79 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="23.8571428571429" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.4285714285714" collapsed="true"/>
+    <col min="3" max="5" customWidth="true" width="22.7142857142857" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.2857142857143" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="32.2857142857143" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -1548,7 +1635,7 @@
         <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1713,7 +1800,7 @@
         <v>40</v>
       </c>
       <c r="I2" t="s">
-        <v>117</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1862,7 +1949,7 @@
         <v>67</v>
       </c>
       <c r="R2" t="s">
-        <v>120</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1937,22 +2024,22 @@
         <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:9">
@@ -1960,25 +2047,25 @@
         <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="E3" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G3" t="s">
         <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2008,13 +2095,13 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D1" t="s">
         <v>17</v>
@@ -2029,7 +2116,7 @@
         <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2037,42 +2124,42 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F2" t="s">
         <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D3" t="s">
         <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -2081,7 +2168,58 @@
         <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>119</v>
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="22.2857142857143" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.5714285714286" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="36.7142857142857" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="24.8571428571429" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding extent spark Report
</commit_message>
<xml_diff>
--- a/ESF/Resources/TestData/Testdata1.xlsx
+++ b/ESF/Resources/TestData/Testdata1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="7665" firstSheet="8" activeTab="11"/>
+    <workbookView windowWidth="28800" windowHeight="12495" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -69,10 +69,10 @@
     <t>atanu</t>
   </si>
   <si>
-    <t>CEE_16959</t>
-  </si>
-  <si>
-    <t>Atanu_Test_544</t>
+    <t>Atanu_Test_318</t>
+  </si>
+  <si>
+    <t>Atanu_Test_387</t>
   </si>
   <si>
     <t>Application Step Name</t>
@@ -120,390 +120,393 @@
     <t>single_column</t>
   </si>
   <si>
+    <t>Atanu_Step_396</t>
+  </si>
+  <si>
+    <t>Section Number</t>
+  </si>
+  <si>
+    <t>Section Name</t>
+  </si>
+  <si>
+    <t>Sequence Number</t>
+  </si>
+  <si>
+    <t>Section Class Name</t>
+  </si>
+  <si>
+    <t>Modified Section Name</t>
+  </si>
+  <si>
+    <t>Test_Section</t>
+  </si>
+  <si>
+    <t>col-mo-12</t>
+  </si>
+  <si>
+    <t>col-mo-6</t>
+  </si>
+  <si>
+    <t>custom-class</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Test_Section_746</t>
+  </si>
+  <si>
+    <t>Unique Id</t>
+  </si>
+  <si>
+    <t>Field Label</t>
+  </si>
+  <si>
+    <t>Field Type</t>
+  </si>
+  <si>
+    <t>Field Sequence</t>
+  </si>
+  <si>
+    <t>Placeholder Text</t>
+  </si>
+  <si>
+    <t>Tooltip</t>
+  </si>
+  <si>
+    <t>Field Character Limit</t>
+  </si>
+  <si>
+    <t>API Key</t>
+  </si>
+  <si>
+    <t>Request API Key</t>
+  </si>
+  <si>
+    <t>Response API Key</t>
+  </si>
+  <si>
+    <t>CSS Class Name</t>
+  </si>
+  <si>
+    <t>Default Value</t>
+  </si>
+  <si>
+    <t>Possible Values</t>
+  </si>
+  <si>
+    <t>Modified Uniq Id</t>
+  </si>
+  <si>
+    <t>user_name</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Textfield</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter Your Username </t>
+  </si>
+  <si>
+    <t>Username needed</t>
+  </si>
+  <si>
+    <t>http#:/#api-key</t>
+  </si>
+  <si>
+    <t>http#:/#Requestapi-key</t>
+  </si>
+  <si>
+    <t>Responseapi-key</t>
+  </si>
+  <si>
+    <t>Bootstrap</t>
+  </si>
+  <si>
+    <t>col-6</t>
+  </si>
+  <si>
+    <t>Comparison Field</t>
+  </si>
+  <si>
+    <t>test_field122</t>
+  </si>
+  <si>
+    <t>user_name_387</t>
+  </si>
+  <si>
+    <t>Condition Name</t>
+  </si>
+  <si>
+    <t>Condition ID</t>
+  </si>
+  <si>
+    <t>Step Name</t>
+  </si>
+  <si>
+    <t>Block Name</t>
+  </si>
+  <si>
+    <t>Field Unique Id</t>
+  </si>
+  <si>
+    <t>Comparison Operator</t>
+  </si>
+  <si>
+    <t>Field Values</t>
+  </si>
+  <si>
+    <t>Api Key</t>
+  </si>
+  <si>
+    <t>Query</t>
+  </si>
+  <si>
+    <t>Modified Condition Id</t>
+  </si>
+  <si>
+    <t>Test_Condition</t>
+  </si>
+  <si>
+    <t>Condition1</t>
+  </si>
+  <si>
+    <t>Atanu_Step_684</t>
+  </si>
+  <si>
+    <t>user_name_275</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>##http/api</t>
+  </si>
+  <si>
+    <t>( Condition1 )</t>
+  </si>
+  <si>
+    <t>Condition2</t>
+  </si>
+  <si>
+    <t>( Condition2 )</t>
+  </si>
+  <si>
+    <t>Application Block Name</t>
+  </si>
+  <si>
+    <t>Block Type</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Modified Block Name</t>
+  </si>
+  <si>
+    <t>genericBlock</t>
+  </si>
+  <si>
+    <t>This is generic block type desc</t>
+  </si>
+  <si>
+    <t>col-mo-10</t>
+  </si>
+  <si>
+    <t>cutom-10-name</t>
+  </si>
+  <si>
+    <t>test_field</t>
+  </si>
+  <si>
+    <t>Atanu_Test_263</t>
+  </si>
+  <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t>This is menu block type desc</t>
+  </si>
+  <si>
+    <t>cutom-10</t>
+  </si>
+  <si>
+    <t>Atanu_Test_629</t>
+  </si>
+  <si>
+    <t>Enter a message code</t>
+  </si>
+  <si>
+    <t>Select a message type</t>
+  </si>
+  <si>
+    <t>Enter the message to be displayed</t>
+  </si>
+  <si>
+    <t>Modified Message Code</t>
+  </si>
+  <si>
+    <t>atanu_test_message</t>
+  </si>
+  <si>
+    <t>Static Message Text</t>
+  </si>
+  <si>
+    <t>This message is for testing perpose</t>
+  </si>
+  <si>
+    <t>atanu_test_message_260</t>
+  </si>
+  <si>
+    <t>Dynamic Message Text</t>
+  </si>
+  <si>
+    <t>atanu_test_message_331</t>
+  </si>
+  <si>
+    <t>Name of the workflow</t>
+  </si>
+  <si>
+    <t>Associate Progress Bar</t>
+  </si>
+  <si>
+    <t>Step Count Color</t>
+  </si>
+  <si>
+    <t>Percentage Text Color</t>
+  </si>
+  <si>
+    <t>Progress Bar Color</t>
+  </si>
+  <si>
+    <t>Modified Workflow Name</t>
+  </si>
+  <si>
+    <t>Test_Workflow</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Test_Workflow_496</t>
+  </si>
+  <si>
+    <t>Modal Id</t>
+  </si>
+  <si>
+    <t>Modal Type</t>
+  </si>
+  <si>
+    <t>Modal Title</t>
+  </si>
+  <si>
+    <t>Icon For Modal Close Button</t>
+  </si>
+  <si>
+    <t>Modal Message Text</t>
+  </si>
+  <si>
+    <t>Enter value for input form fields</t>
+  </si>
+  <si>
+    <t>Button Label</t>
+  </si>
+  <si>
+    <t>Button Type</t>
+  </si>
+  <si>
+    <t>Link Event</t>
+  </si>
+  <si>
+    <t>Modified Modal Id</t>
+  </si>
+  <si>
+    <t>Test_Modal</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
+    <t>testModal</t>
+  </si>
+  <si>
+    <t>closeicon</t>
+  </si>
+  <si>
+    <t>Warning!! This is for testing purpose</t>
+  </si>
+  <si>
+    <t>btnLabel</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Test_Modal_368</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Validation Message Type</t>
+  </si>
+  <si>
+    <t>Display Type</t>
+  </si>
+  <si>
+    <t>Associate Message Code</t>
+  </si>
+  <si>
+    <t>Modified Name</t>
+  </si>
+  <si>
+    <t>Conditional ID</t>
+  </si>
+  <si>
+    <t>CompareBy</t>
+  </si>
+  <si>
+    <t>Condition Query</t>
+  </si>
+  <si>
+    <t>Expected Validation Message Type</t>
+  </si>
+  <si>
+    <t>Test_Validation</t>
+  </si>
+  <si>
+    <t>Mandatory</t>
+  </si>
+  <si>
+    <t>Inline</t>
+  </si>
+  <si>
+    <t>Test_Validation_737</t>
+  </si>
+  <si>
+    <t>|- None -|Mandatory|Regex|Conditional|Individual File Size|Total File Size|File Type</t>
+  </si>
+  <si>
+    <t>Conditional</t>
+  </si>
+  <si>
+    <t>Test_Validation_22</t>
+  </si>
+  <si>
+    <t>Condition3</t>
+  </si>
+  <si>
     <t>Atanu_Step_716</t>
   </si>
   <si>
-    <t>Section Number</t>
-  </si>
-  <si>
-    <t>Section Name</t>
-  </si>
-  <si>
-    <t>Sequence Number</t>
-  </si>
-  <si>
-    <t>Section Class Name</t>
-  </si>
-  <si>
-    <t>Modified Section Name</t>
-  </si>
-  <si>
-    <t>Test_Section</t>
-  </si>
-  <si>
-    <t>col-mo-12</t>
-  </si>
-  <si>
-    <t>col-mo-6</t>
-  </si>
-  <si>
-    <t>custom-class</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>Test_Section_746</t>
-  </si>
-  <si>
-    <t>Unique Id</t>
-  </si>
-  <si>
-    <t>Field Label</t>
-  </si>
-  <si>
-    <t>Field Type</t>
-  </si>
-  <si>
-    <t>Field Sequence</t>
-  </si>
-  <si>
-    <t>Placeholder Text</t>
-  </si>
-  <si>
-    <t>Tooltip</t>
-  </si>
-  <si>
-    <t>Field Character Limit</t>
-  </si>
-  <si>
-    <t>API Key</t>
-  </si>
-  <si>
-    <t>Request API Key</t>
-  </si>
-  <si>
-    <t>Response API Key</t>
-  </si>
-  <si>
-    <t>CSS Class Name</t>
-  </si>
-  <si>
-    <t>Default Value</t>
-  </si>
-  <si>
-    <t>Possible Values</t>
-  </si>
-  <si>
-    <t>Modified Uniq Id</t>
-  </si>
-  <si>
-    <t>user_name</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Textfield</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enter Your Username </t>
-  </si>
-  <si>
-    <t>Username needed</t>
-  </si>
-  <si>
-    <t>http#:/#api-key</t>
-  </si>
-  <si>
-    <t>http#:/#Requestapi-key</t>
-  </si>
-  <si>
-    <t>Responseapi-key</t>
-  </si>
-  <si>
-    <t>Bootstrap</t>
-  </si>
-  <si>
-    <t>col-6</t>
-  </si>
-  <si>
-    <t>Comparison Field</t>
-  </si>
-  <si>
-    <t>test_field122</t>
-  </si>
-  <si>
-    <t>user_name_387</t>
-  </si>
-  <si>
-    <t>Condition Name</t>
-  </si>
-  <si>
-    <t>Condition ID</t>
-  </si>
-  <si>
-    <t>Step Name</t>
-  </si>
-  <si>
-    <t>Block Name</t>
-  </si>
-  <si>
-    <t>Field Unique Id</t>
-  </si>
-  <si>
-    <t>Comparison Operator</t>
-  </si>
-  <si>
-    <t>Field Values</t>
-  </si>
-  <si>
-    <t>Api Key</t>
-  </si>
-  <si>
-    <t>Query</t>
-  </si>
-  <si>
-    <t>Modified Condition Id</t>
-  </si>
-  <si>
-    <t>Test_Condition</t>
-  </si>
-  <si>
-    <t>Condition1</t>
-  </si>
-  <si>
-    <t>Atanu_Step_684</t>
-  </si>
-  <si>
-    <t>user_name_275</t>
-  </si>
-  <si>
-    <t>NE</t>
-  </si>
-  <si>
-    <t>##http/api</t>
-  </si>
-  <si>
-    <t>( Condition1 )</t>
-  </si>
-  <si>
-    <t>Condition2</t>
-  </si>
-  <si>
-    <t>( Condition2 )</t>
-  </si>
-  <si>
-    <t>Application Block Name</t>
-  </si>
-  <si>
-    <t>Block Type</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Modified Block Name</t>
-  </si>
-  <si>
-    <t>genericBlock</t>
-  </si>
-  <si>
-    <t>This is generic block type desc</t>
-  </si>
-  <si>
-    <t>col-mo-10</t>
-  </si>
-  <si>
-    <t>cutom-10-name</t>
-  </si>
-  <si>
-    <t>test_field</t>
-  </si>
-  <si>
-    <t>Atanu_Test_263</t>
-  </si>
-  <si>
-    <t>menu</t>
-  </si>
-  <si>
-    <t>This is menu block type desc</t>
-  </si>
-  <si>
-    <t>cutom-10</t>
-  </si>
-  <si>
-    <t>Atanu_Test_629</t>
-  </si>
-  <si>
-    <t>Enter a message code</t>
-  </si>
-  <si>
-    <t>Select a message type</t>
-  </si>
-  <si>
-    <t>Enter the message to be displayed</t>
-  </si>
-  <si>
-    <t>Modified Message Code</t>
-  </si>
-  <si>
-    <t>atanu_test_message</t>
-  </si>
-  <si>
-    <t>Static Message Text</t>
-  </si>
-  <si>
-    <t>This message is for testing perpose</t>
-  </si>
-  <si>
-    <t>atanu_test_message_240</t>
-  </si>
-  <si>
-    <t>Dynamic Message Text</t>
-  </si>
-  <si>
-    <t>atanu_test_message_788</t>
-  </si>
-  <si>
-    <t>Name of the workflow</t>
-  </si>
-  <si>
-    <t>Associate Progress Bar</t>
-  </si>
-  <si>
-    <t>Step Count Color</t>
-  </si>
-  <si>
-    <t>Percentage Text Color</t>
-  </si>
-  <si>
-    <t>Progress Bar Color</t>
-  </si>
-  <si>
-    <t>Modified Workflow Name</t>
-  </si>
-  <si>
-    <t>Test_Workflow</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>Blue</t>
-  </si>
-  <si>
-    <t>Black</t>
-  </si>
-  <si>
-    <t>Test_Workflow_496</t>
-  </si>
-  <si>
-    <t>Modal Id</t>
-  </si>
-  <si>
-    <t>Modal Type</t>
-  </si>
-  <si>
-    <t>Modal Title</t>
-  </si>
-  <si>
-    <t>Icon For Modal Close Button</t>
-  </si>
-  <si>
-    <t>Modal Message Text</t>
-  </si>
-  <si>
-    <t>Enter value for input form fields</t>
-  </si>
-  <si>
-    <t>Button Label</t>
-  </si>
-  <si>
-    <t>Button Type</t>
-  </si>
-  <si>
-    <t>Link Event</t>
-  </si>
-  <si>
-    <t>Modified Modal Id</t>
-  </si>
-  <si>
-    <t>Test_Modal</t>
-  </si>
-  <si>
-    <t>Info</t>
-  </si>
-  <si>
-    <t>testModal</t>
-  </si>
-  <si>
-    <t>closeicon</t>
-  </si>
-  <si>
-    <t>Warning!! This is for testing purpose</t>
-  </si>
-  <si>
-    <t>btnLabel</t>
-  </si>
-  <si>
-    <t>Positive</t>
-  </si>
-  <si>
-    <t>Test_Modal_368</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Validation Message Type</t>
-  </si>
-  <si>
-    <t>Display Type</t>
-  </si>
-  <si>
-    <t>Associate Message Code</t>
-  </si>
-  <si>
-    <t>Modified Name</t>
-  </si>
-  <si>
-    <t>Conditional ID</t>
-  </si>
-  <si>
-    <t>CompareBy</t>
-  </si>
-  <si>
-    <t>Condition Query</t>
-  </si>
-  <si>
-    <t>Expected Validation Message Type</t>
-  </si>
-  <si>
-    <t>Test_Validation</t>
-  </si>
-  <si>
-    <t>Mandatory</t>
-  </si>
-  <si>
-    <t>Inline</t>
-  </si>
-  <si>
-    <t>Test_Validation_737</t>
-  </si>
-  <si>
-    <t>|- None -|Mandatory|Regex|Conditional|Individual File Size|Total File Size|File Type</t>
-  </si>
-  <si>
-    <t>Conditional</t>
-  </si>
-  <si>
-    <t>Test_Validation_705</t>
-  </si>
-  <si>
-    <t>Condition3</t>
-  </si>
-  <si>
     <t>!=</t>
   </si>
   <si>
@@ -514,9 +517,6 @@
   </si>
   <si>
     <t>( Condition3 )</t>
-  </si>
-  <si>
-    <t>Test_Validation_31</t>
   </si>
 </sst>
 </file>
@@ -525,9 +525,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -560,6 +560,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -569,29 +576,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -644,8 +643,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -658,9 +666,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -675,14 +682,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -697,43 +697,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -745,139 +877,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -906,11 +906,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -954,17 +960,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -993,49 +993,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1047,94 +1047,94 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1490,8 +1490,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="27.7142857142857" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.5714285714286" collapsed="true"/>
+    <col min="1" max="1" width="27.7142857142857" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.5714285714286" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1527,11 +1527,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.8571428571429" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.4285714285714" collapsed="true"/>
-    <col min="3" max="5" customWidth="true" width="22.7142857142857" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="20.2857142857143" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="32.2857142857143" collapsed="true"/>
+    <col min="1" max="1" width="23.8571428571429" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.4285714285714" customWidth="1" collapsed="1"/>
+    <col min="3" max="5" width="22.7142857142857" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.2857142857143" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="32.2857142857143" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1594,16 +1594,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.7142857142857" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.8571428571429" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="30.1428571428571" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="32.8571428571429" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="29.5714285714286" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="17.7142857142857" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="17.8571428571429" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="17.5714285714286" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="28.1428571428571" collapsed="true"/>
+    <col min="1" max="1" width="16.7142857142857" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.8571428571429" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="30.1428571428571" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.8571428571429" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29.5714285714286" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.7142857142857" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.8571428571429" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.5714285714286" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="28.1428571428571" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1678,25 +1678,25 @@
   <sheetPr/>
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="24.0" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="21.4285714285714" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="28.1428571428571" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="26.0" collapsed="false"/>
-    <col min="6" max="7" customWidth="true" width="18.7142857142857" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="17.5714285714286" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="22.2857142857143" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="18.4285714285714" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="16.5714285714286" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" width="19.1428571428571" collapsed="false"/>
-    <col min="13" max="13" customWidth="true" width="19.0" collapsed="false"/>
-    <col min="14" max="14" customWidth="true" width="77.2857142857143" collapsed="false"/>
+    <col min="1" max="1" width="20" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.4285714285714" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="28.1428571428571" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="18.7142857142857" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.5714285714286" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="22.2857142857143" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.4285714285714" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.5714285714286" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="19.1428571428571" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="19" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="77.2857142857143" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1777,31 +1777,31 @@
         <v>112</v>
       </c>
       <c r="E3" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>158</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>159</v>
       </c>
       <c r="H3" t="s">
         <v>69</v>
       </c>
       <c r="I3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="J3" t="s">
         <v>41</v>
       </c>
       <c r="K3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="L3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="N3" t="s">
         <v>155</v>
@@ -1819,17 +1819,17 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.7142857142857" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.5714285714286" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="21.1428571428571" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.2857142857143" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="34.4285714285714" collapsed="true"/>
+    <col min="1" max="1" width="22.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="18.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="21.1428571428571" customWidth="1"/>
+    <col min="5" max="5" width="19.2857142857143" customWidth="1"/>
+    <col min="6" max="6" width="34.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="1" spans="1:6">
@@ -1903,21 +1903,21 @@
   <sheetPr/>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.2857142857143" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="27.4285714285714" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="21.4285714285714" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.8571428571429" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="25.2857142857143" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="18.8571428571429" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="19.8571428571429" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="27.4285714285714" collapsed="true"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="21.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="27.4285714285714" customWidth="1"/>
+    <col min="4" max="4" width="21.4285714285714" customWidth="1"/>
+    <col min="5" max="5" width="19.8571428571429" customWidth="1"/>
+    <col min="6" max="6" width="25.2857142857143" customWidth="1"/>
+    <col min="7" max="7" width="18.8571428571429" customWidth="1"/>
+    <col min="8" max="8" width="19.8571428571429" customWidth="1"/>
+    <col min="9" max="9" width="27.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="1" ht="17.25" spans="1:9">
@@ -1998,7 +1998,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="37.7142857142857" collapsed="true"/>
+    <col min="1" max="1" width="37.7142857142857" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -2006,8 +2006,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" ht="17.25" spans="1:1">
-      <c r="A2" s="3"/>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" ht="17.25" spans="1:1">
       <c r="A3" s="3"/>
@@ -2074,15 +2076,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="22.2857142857143" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="24.2857142857143" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="27.5714285714286" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="27.1428571428571" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="18.5714285714286" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="27.2857142857143" collapsed="true"/>
+    <col min="1" max="1" width="15" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.2857142857143" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.2857142857143" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27.5714285714286" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.1428571428571" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.5714285714286" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="27.2857142857143" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" spans="1:9">
@@ -2160,24 +2162,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.1428571428571" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.2857142857143" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="25.8571428571429" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.5714285714286" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="19.1428571428571" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="26.5714285714286" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="24.2857142857143" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="27.7142857142857" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="23.4285714285714" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="19.8571428571429" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="24.1428571428571" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="18.4285714285714" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="19.8571428571429" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="27.7142857142857" collapsed="true"/>
+    <col min="1" max="1" width="17.1428571428571" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.2857142857143" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="25.8571428571429" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.5714285714286" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.1428571428571" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="26.5714285714286" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.2857142857143" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="27.7142857142857" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.4285714285714" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="19" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="19.8571428571429" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="20" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="24.1428571428571" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="18.4285714285714" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="19.8571428571429" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="27.7142857142857" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -2312,16 +2314,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.4285714285714" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="20.1428571428571" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="21.5714285714286" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="20.8571428571429" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="27.2857142857143" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="24.2857142857143" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="18.7142857142857" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="22.7142857142857" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="31.4285714285714" collapsed="true"/>
+    <col min="1" max="1" width="20.4285714285714" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.1428571428571" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.5714285714286" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.8571428571429" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.2857142857143" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="24.2857142857143" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.7142857142857" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="22.7142857142857" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="31.4285714285714" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2425,12 +2427,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.7142857142857" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="27.1428571428571" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="36.4285714285714" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="6" max="7" customWidth="true" width="28.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="33.8571428571429" collapsed="true"/>
+    <col min="1" max="1" width="22.7142857142857" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.1428571428571" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="36.4285714285714" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="27" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="28" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="33.8571428571429" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2528,10 +2530,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.2857142857143" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="22.5714285714286" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="36.7142857142857" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="24.8571428571429" collapsed="false"/>
+    <col min="1" max="1" width="22.2857142857143" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.5714285714286" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="36.7142857142857" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.8571428571429" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>